<commit_message>
finished the bulk of it. debugging tomorrow
</commit_message>
<xml_diff>
--- a/projects/cs2200-project-1/microcode/microcode.xlsx
+++ b/projects/cs2200-project-1/microcode/microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruh\Documents\GT\Fall 2023\CS_2200\projects\cs2200-project-1\microcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9C16C7-1693-4ABF-8E42-5A1A0CEB7F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0601B6-958F-49D3-80E4-93055523C34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
   <si>
     <t>Index</t>
   </si>
@@ -215,12 +215,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>0000</t>
   </si>
   <si>
@@ -303,6 +297,123 @@
   </si>
   <si>
     <t>add3</t>
+  </si>
+  <si>
+    <t>nand1</t>
+  </si>
+  <si>
+    <t>nand2</t>
+  </si>
+  <si>
+    <t>nand3</t>
+  </si>
+  <si>
+    <t>addi1</t>
+  </si>
+  <si>
+    <t>addi2</t>
+  </si>
+  <si>
+    <t>addi3</t>
+  </si>
+  <si>
+    <t>lw1</t>
+  </si>
+  <si>
+    <t>lw2</t>
+  </si>
+  <si>
+    <t>lw3</t>
+  </si>
+  <si>
+    <t>lw4</t>
+  </si>
+  <si>
+    <t>sw1</t>
+  </si>
+  <si>
+    <t>sw2</t>
+  </si>
+  <si>
+    <t>sw3</t>
+  </si>
+  <si>
+    <t>sw4</t>
+  </si>
+  <si>
+    <t>beq1</t>
+  </si>
+  <si>
+    <t>beq2</t>
+  </si>
+  <si>
+    <t>beq3</t>
+  </si>
+  <si>
+    <t>beq4</t>
+  </si>
+  <si>
+    <t>beq5</t>
+  </si>
+  <si>
+    <t>beq6</t>
+  </si>
+  <si>
+    <t>jalr1</t>
+  </si>
+  <si>
+    <t>jalr2</t>
+  </si>
+  <si>
+    <t>halt</t>
+  </si>
+  <si>
+    <t>blt1</t>
+  </si>
+  <si>
+    <t>blt2</t>
+  </si>
+  <si>
+    <t>blt3</t>
+  </si>
+  <si>
+    <t>blt4</t>
+  </si>
+  <si>
+    <t>lea1</t>
+  </si>
+  <si>
+    <t>lea2</t>
+  </si>
+  <si>
+    <t>lea3</t>
+  </si>
+  <si>
+    <t>bgt1</t>
+  </si>
+  <si>
+    <t>bgt2</t>
+  </si>
+  <si>
+    <t>bgt3</t>
+  </si>
+  <si>
+    <t>bgt4</t>
+  </si>
+  <si>
+    <t>or1</t>
+  </si>
+  <si>
+    <t>or2</t>
+  </si>
+  <si>
+    <t>or3</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>000000</t>
   </si>
 </sst>
 </file>
@@ -560,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,6 +778,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -934,9 +1052,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP997"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V9" sqref="V9"/>
+      <selection pane="bottomLeft" activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -1057,7 +1175,7 @@
       <c r="AP1" s="1"/>
     </row>
     <row r="2" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="40">
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1153,7 +1271,7 @@
       </c>
     </row>
     <row r="3" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1249,7 +1367,7 @@
       </c>
     </row>
     <row r="4" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A4" s="4">
+      <c r="A4" s="40">
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -1259,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -1275,7 +1393,7 @@
       </c>
       <c r="I4" s="5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
@@ -1341,16 +1459,16 @@
       <c r="AE4" s="4"/>
       <c r="AF4" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1C01110</v>
+        <v>1C01100</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A5" s="4">
+    <row r="5" spans="1:42" ht="13.8" customHeight="1">
+      <c r="A5" s="40">
         <f t="shared" ref="A5:A49" si="3">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -1417,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="X5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="2">
         <v>0</v>
@@ -1438,16 +1556,16 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0208044</v>
+        <v>0108044</v>
       </c>
     </row>
     <row r="6" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="40">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1514,10 +1632,10 @@
         <v>0</v>
       </c>
       <c r="X6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="2">
         <v>0</v>
@@ -1535,16 +1653,16 @@
       <c r="AE6" s="4"/>
       <c r="AF6" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0110045</v>
+        <v>0210045</v>
       </c>
     </row>
     <row r="7" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A7" s="4">
+      <c r="A7" s="40">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -1636,11 +1754,13 @@
       </c>
     </row>
     <row r="8" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A8" s="4">
+      <c r="A8" s="40">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
@@ -1651,20 +1771,20 @@
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -1691,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="2">
         <v>0</v>
@@ -1706,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="2">
         <v>0</v>
@@ -1727,15 +1847,17 @@
       <c r="AE8" s="4"/>
       <c r="AF8" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0108047</v>
       </c>
     </row>
     <row r="9" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A9" s="4">
+      <c r="A9" s="40">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
@@ -1743,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -1756,10 +1878,10 @@
       </c>
       <c r="I9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -1789,7 +1911,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="2">
         <v>0</v>
@@ -1804,7 +1926,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9" s="2">
         <v>0</v>
@@ -1822,15 +1944,17 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0210048</v>
       </c>
     </row>
     <row r="10" spans="1:42" ht="14.25" customHeight="1">
-      <c r="A10" s="4">
+      <c r="A10" s="40">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="C10" s="2">
         <v>0</v>
       </c>
@@ -1860,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="2">
         <v>0</v>
@@ -1890,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="2">
         <v>0</v>
@@ -1905,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" s="2">
         <v>0</v>
@@ -1917,7 +2041,7 @@
       <c r="AE10" s="4"/>
       <c r="AF10" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0840100</v>
       </c>
     </row>
     <row r="11" spans="1:42" ht="14.25" customHeight="1">
@@ -1925,7 +2049,9 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="C11" s="2">
         <v>0</v>
       </c>
@@ -1933,20 +2059,20 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J11" s="2">
         <v>0</v>
@@ -1964,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="O11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="2">
         <v>0</v>
@@ -1976,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="2">
         <v>0</v>
@@ -2012,7 +2138,7 @@
       <c r="AE11" s="4"/>
       <c r="AF11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>000880A</v>
       </c>
     </row>
     <row r="12" spans="1:42" ht="14.25" customHeight="1">
@@ -2020,7 +2146,9 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="C12" s="2">
         <v>0</v>
       </c>
@@ -2028,23 +2156,23 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
@@ -2074,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="2">
         <v>0</v>
@@ -2086,7 +2214,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y12" s="2">
         <v>0</v>
@@ -2107,7 +2235,7 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>011004B</v>
       </c>
     </row>
     <row r="13" spans="1:42" ht="14.25" customHeight="1">
@@ -2115,7 +2243,9 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="C13" s="2">
         <v>0</v>
       </c>
@@ -2145,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
@@ -2175,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="2">
         <v>0</v>
@@ -2202,7 +2332,7 @@
       <c r="AE13" s="4"/>
       <c r="AF13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0040100</v>
       </c>
     </row>
     <row r="14" spans="1:42" ht="14.25" customHeight="1">
@@ -2210,7 +2340,9 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C14" s="2">
         <v>0</v>
       </c>
@@ -2218,20 +2350,20 @@
         <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J14" s="2">
         <v>0</v>
@@ -2249,7 +2381,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="2">
         <v>0</v>
@@ -2261,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14" s="2">
         <v>0</v>
@@ -2297,7 +2429,7 @@
       <c r="AE14" s="4"/>
       <c r="AF14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>000880D</v>
       </c>
     </row>
     <row r="15" spans="1:42" ht="14.25" customHeight="1">
@@ -2305,7 +2437,9 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="C15" s="2">
         <v>0</v>
       </c>
@@ -2313,23 +2447,23 @@
         <v>0</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
@@ -2359,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="2">
         <v>0</v>
@@ -2371,7 +2505,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="2">
         <v>0</v>
@@ -2392,7 +2526,7 @@
       <c r="AE15" s="4"/>
       <c r="AF15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>011004E</v>
       </c>
     </row>
     <row r="16" spans="1:42" ht="14.25" customHeight="1">
@@ -2400,7 +2534,9 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C16" s="2">
         <v>0</v>
       </c>
@@ -2408,20 +2544,20 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J16" s="2">
         <v>0</v>
@@ -2430,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="2">
         <v>0</v>
@@ -2448,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" s="2">
         <v>0</v>
@@ -2487,7 +2623,7 @@
       <c r="AE16" s="4"/>
       <c r="AF16" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>000410F</v>
       </c>
     </row>
     <row r="17" spans="1:32" ht="14.25" customHeight="1">
@@ -2495,7 +2631,9 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
@@ -2522,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
@@ -2555,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="2">
         <v>0</v>
@@ -2582,7 +2720,7 @@
       <c r="AE17" s="4"/>
       <c r="AF17" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0040080</v>
       </c>
     </row>
     <row r="18" spans="1:32" ht="14.25" customHeight="1">
@@ -2590,12 +2728,14 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -2607,11 +2747,11 @@
         <v>0</v>
       </c>
       <c r="H18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J18" s="2">
         <v>0</v>
@@ -2629,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
@@ -2641,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="2">
         <v>0</v>
@@ -2677,7 +2817,7 @@
       <c r="AE18" s="4"/>
       <c r="AF18" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0008811</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="14.25" customHeight="1">
@@ -2685,12 +2825,14 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="C19" s="2">
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -2699,17 +2841,17 @@
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="2">
         <v>0</v>
@@ -2739,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="T19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="2">
         <v>0</v>
@@ -2751,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="2">
         <v>0</v>
@@ -2772,7 +2914,7 @@
       <c r="AE19" s="4"/>
       <c r="AF19" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0110052</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="14.25" customHeight="1">
@@ -2780,12 +2922,14 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="C20" s="2">
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -2794,14 +2938,14 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J20" s="2">
         <v>0</v>
@@ -2810,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="2">
         <v>0</v>
@@ -2828,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="2">
         <v>0</v>
@@ -2867,15 +3011,17 @@
       <c r="AE20" s="4"/>
       <c r="AF20" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0004113</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="14.25" customHeight="1">
+    <row r="21" spans="1:32" ht="13.8" customHeight="1">
       <c r="A21" s="4">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="C21" s="2">
         <v>0</v>
       </c>
@@ -2899,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
@@ -2938,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="W21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21" s="2">
         <v>0</v>
@@ -2962,577 +3108,589 @@
       <c r="AE21" s="4"/>
       <c r="AF21" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0080040</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A22" s="4">
+      <c r="A22" s="40">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
+      <c r="B22" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="41">
+        <v>0</v>
+      </c>
+      <c r="D22" s="41">
+        <v>1</v>
+      </c>
+      <c r="E22" s="41">
+        <v>0</v>
+      </c>
+      <c r="F22" s="41">
+        <v>1</v>
+      </c>
+      <c r="G22" s="41">
+        <v>0</v>
+      </c>
+      <c r="H22" s="41">
+        <v>1</v>
       </c>
       <c r="I22" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0</v>
-      </c>
-      <c r="N22" s="2">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>0</v>
-      </c>
-      <c r="R22" s="2">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2">
-        <v>0</v>
-      </c>
-      <c r="T22" s="2">
-        <v>0</v>
-      </c>
-      <c r="U22" s="2">
-        <v>0</v>
-      </c>
-      <c r="V22" s="2">
-        <v>0</v>
-      </c>
-      <c r="W22" s="2">
-        <v>0</v>
-      </c>
-      <c r="X22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="J22" s="41">
+        <v>1</v>
+      </c>
+      <c r="K22" s="41">
+        <v>0</v>
+      </c>
+      <c r="L22" s="41">
+        <v>0</v>
+      </c>
+      <c r="M22" s="41">
+        <v>0</v>
+      </c>
+      <c r="N22" s="41">
+        <v>0</v>
+      </c>
+      <c r="O22" s="41">
+        <v>0</v>
+      </c>
+      <c r="P22" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="41">
+        <v>0</v>
+      </c>
+      <c r="R22" s="41">
+        <v>0</v>
+      </c>
+      <c r="S22" s="41">
+        <v>1</v>
+      </c>
+      <c r="T22" s="41">
+        <v>0</v>
+      </c>
+      <c r="U22" s="41">
+        <v>0</v>
+      </c>
+      <c r="V22" s="41">
+        <v>0</v>
+      </c>
+      <c r="W22" s="41">
+        <v>0</v>
+      </c>
+      <c r="X22" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="42">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="40"/>
       <c r="AE22" s="4"/>
       <c r="AF22" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0008055</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A23" s="4">
+      <c r="A23" s="40">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
+      <c r="B23" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="41">
+        <v>0</v>
+      </c>
+      <c r="D23" s="41">
+        <v>1</v>
+      </c>
+      <c r="E23" s="41">
+        <v>0</v>
+      </c>
+      <c r="F23" s="41">
+        <v>1</v>
+      </c>
+      <c r="G23" s="41">
+        <v>1</v>
+      </c>
+      <c r="H23" s="41">
         <v>0</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0</v>
-      </c>
-      <c r="N23" s="2">
-        <v>0</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0</v>
-      </c>
-      <c r="S23" s="2">
-        <v>0</v>
-      </c>
-      <c r="T23" s="2">
-        <v>0</v>
-      </c>
-      <c r="U23" s="2">
-        <v>0</v>
-      </c>
-      <c r="V23" s="2">
-        <v>0</v>
-      </c>
-      <c r="W23" s="2">
-        <v>0</v>
-      </c>
-      <c r="X23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="J23" s="41">
+        <v>1</v>
+      </c>
+      <c r="K23" s="41">
+        <v>0</v>
+      </c>
+      <c r="L23" s="41">
+        <v>0</v>
+      </c>
+      <c r="M23" s="41">
+        <v>0</v>
+      </c>
+      <c r="N23" s="41">
+        <v>0</v>
+      </c>
+      <c r="O23" s="41">
+        <v>0</v>
+      </c>
+      <c r="P23" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="41">
+        <v>0</v>
+      </c>
+      <c r="R23" s="41">
+        <v>0</v>
+      </c>
+      <c r="S23" s="41">
+        <v>0</v>
+      </c>
+      <c r="T23" s="41">
+        <v>1</v>
+      </c>
+      <c r="U23" s="41">
+        <v>0</v>
+      </c>
+      <c r="V23" s="41">
+        <v>0</v>
+      </c>
+      <c r="W23" s="41">
+        <v>0</v>
+      </c>
+      <c r="X23" s="41">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="42">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="40"/>
       <c r="AE23" s="4"/>
       <c r="AF23" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0110056</v>
       </c>
     </row>
     <row r="24" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A24" s="4">
+      <c r="A24" s="40">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
+      <c r="B24" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="41">
+        <v>0</v>
+      </c>
+      <c r="D24" s="41">
+        <v>1</v>
+      </c>
+      <c r="E24" s="41">
+        <v>0</v>
+      </c>
+      <c r="F24" s="41">
+        <v>1</v>
+      </c>
+      <c r="G24" s="41">
+        <v>1</v>
+      </c>
+      <c r="H24" s="41">
+        <v>1</v>
       </c>
       <c r="I24" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0</v>
-      </c>
-      <c r="M24" s="2">
-        <v>0</v>
-      </c>
-      <c r="N24" s="2">
-        <v>0</v>
-      </c>
-      <c r="O24" s="2">
-        <v>0</v>
-      </c>
-      <c r="P24" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>0</v>
-      </c>
-      <c r="R24" s="2">
-        <v>0</v>
-      </c>
-      <c r="S24" s="2">
-        <v>0</v>
-      </c>
-      <c r="T24" s="2">
-        <v>0</v>
-      </c>
-      <c r="U24" s="2">
-        <v>0</v>
-      </c>
-      <c r="V24" s="2">
-        <v>0</v>
-      </c>
-      <c r="W24" s="2">
-        <v>0</v>
-      </c>
-      <c r="X24" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA24" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="J24" s="41">
+        <v>0</v>
+      </c>
+      <c r="K24" s="41">
+        <v>0</v>
+      </c>
+      <c r="L24" s="41">
+        <v>1</v>
+      </c>
+      <c r="M24" s="41">
+        <v>0</v>
+      </c>
+      <c r="N24" s="41">
+        <v>0</v>
+      </c>
+      <c r="O24" s="41">
+        <v>0</v>
+      </c>
+      <c r="P24" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="41">
+        <v>0</v>
+      </c>
+      <c r="R24" s="41">
+        <v>0</v>
+      </c>
+      <c r="S24" s="41">
+        <v>0</v>
+      </c>
+      <c r="T24" s="41">
+        <v>0</v>
+      </c>
+      <c r="U24" s="41">
+        <v>1</v>
+      </c>
+      <c r="V24" s="41">
+        <v>0</v>
+      </c>
+      <c r="W24" s="41">
+        <v>0</v>
+      </c>
+      <c r="X24" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="41">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="42">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="40"/>
       <c r="AE24" s="4"/>
       <c r="AF24" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>2420117</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A25" s="4">
+      <c r="A25" s="40">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="B25" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="41">
+        <v>0</v>
+      </c>
+      <c r="D25" s="41">
+        <v>1</v>
+      </c>
+      <c r="E25" s="41">
+        <v>1</v>
+      </c>
+      <c r="F25" s="41">
+        <v>0</v>
+      </c>
+      <c r="G25" s="41">
+        <v>0</v>
+      </c>
+      <c r="H25" s="41">
         <v>0</v>
       </c>
       <c r="I25" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <v>0</v>
-      </c>
-      <c r="L25" s="2">
-        <v>0</v>
-      </c>
-      <c r="M25" s="2">
-        <v>0</v>
-      </c>
-      <c r="N25" s="2">
-        <v>0</v>
-      </c>
-      <c r="O25" s="2">
-        <v>0</v>
-      </c>
-      <c r="P25" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>0</v>
-      </c>
-      <c r="R25" s="2">
-        <v>0</v>
-      </c>
-      <c r="S25" s="2">
-        <v>0</v>
-      </c>
-      <c r="T25" s="2">
-        <v>0</v>
-      </c>
-      <c r="U25" s="2">
-        <v>0</v>
-      </c>
-      <c r="V25" s="2">
-        <v>0</v>
-      </c>
-      <c r="W25" s="2">
-        <v>0</v>
-      </c>
-      <c r="X25" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD25" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="J25" s="41">
+        <v>0</v>
+      </c>
+      <c r="K25" s="41">
+        <v>0</v>
+      </c>
+      <c r="L25" s="41">
+        <v>0</v>
+      </c>
+      <c r="M25" s="41">
+        <v>0</v>
+      </c>
+      <c r="N25" s="41">
+        <v>1</v>
+      </c>
+      <c r="O25" s="41">
+        <v>0</v>
+      </c>
+      <c r="P25" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="41">
+        <v>0</v>
+      </c>
+      <c r="R25" s="41">
+        <v>0</v>
+      </c>
+      <c r="S25" s="41">
+        <v>1</v>
+      </c>
+      <c r="T25" s="41">
+        <v>0</v>
+      </c>
+      <c r="U25" s="41">
+        <v>0</v>
+      </c>
+      <c r="V25" s="41">
+        <v>0</v>
+      </c>
+      <c r="W25" s="41">
+        <v>0</v>
+      </c>
+      <c r="X25" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="42">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="40"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0008418</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A26" s="4">
+      <c r="A26" s="40">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0</v>
+      <c r="B26" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="41">
+        <v>0</v>
+      </c>
+      <c r="D26" s="41">
+        <v>1</v>
+      </c>
+      <c r="E26" s="41">
+        <v>1</v>
+      </c>
+      <c r="F26" s="41">
+        <v>0</v>
+      </c>
+      <c r="G26" s="41">
+        <v>0</v>
+      </c>
+      <c r="H26" s="41">
+        <v>1</v>
       </c>
       <c r="I26" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0</v>
-      </c>
-      <c r="N26" s="2">
-        <v>0</v>
-      </c>
-      <c r="O26" s="2">
-        <v>0</v>
-      </c>
-      <c r="P26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>0</v>
-      </c>
-      <c r="R26" s="2">
-        <v>0</v>
-      </c>
-      <c r="S26" s="2">
-        <v>0</v>
-      </c>
-      <c r="T26" s="2">
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <v>0</v>
-      </c>
-      <c r="V26" s="2">
-        <v>0</v>
-      </c>
-      <c r="W26" s="2">
-        <v>0</v>
-      </c>
-      <c r="X26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="18">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="J26" s="41">
+        <v>0</v>
+      </c>
+      <c r="K26" s="41">
+        <v>0</v>
+      </c>
+      <c r="L26" s="41">
+        <v>0</v>
+      </c>
+      <c r="M26" s="41">
+        <v>0</v>
+      </c>
+      <c r="N26" s="41">
+        <v>0</v>
+      </c>
+      <c r="O26" s="41">
+        <v>1</v>
+      </c>
+      <c r="P26" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="41">
+        <v>0</v>
+      </c>
+      <c r="R26" s="41">
+        <v>0</v>
+      </c>
+      <c r="S26" s="41">
+        <v>0</v>
+      </c>
+      <c r="T26" s="41">
+        <v>1</v>
+      </c>
+      <c r="U26" s="41">
+        <v>0</v>
+      </c>
+      <c r="V26" s="41">
+        <v>0</v>
+      </c>
+      <c r="W26" s="41">
+        <v>0</v>
+      </c>
+      <c r="X26" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="42">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="40"/>
       <c r="AE26" s="4"/>
       <c r="AF26" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0010819</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="14.25" customHeight="1">
-      <c r="A27" s="4">
+      <c r="A27" s="40">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0</v>
-      </c>
-      <c r="H27" s="2">
+      <c r="B27" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="41">
+        <v>0</v>
+      </c>
+      <c r="D27" s="41">
+        <v>0</v>
+      </c>
+      <c r="E27" s="41">
+        <v>0</v>
+      </c>
+      <c r="F27" s="41">
+        <v>0</v>
+      </c>
+      <c r="G27" s="41">
+        <v>0</v>
+      </c>
+      <c r="H27" s="41">
         <v>0</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J27" s="2">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2">
-        <v>0</v>
-      </c>
-      <c r="M27" s="2">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2">
-        <v>0</v>
-      </c>
-      <c r="O27" s="2">
-        <v>0</v>
-      </c>
-      <c r="P27" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>0</v>
-      </c>
-      <c r="R27" s="2">
-        <v>0</v>
-      </c>
-      <c r="S27" s="2">
-        <v>0</v>
-      </c>
-      <c r="T27" s="2">
-        <v>0</v>
-      </c>
-      <c r="U27" s="2">
-        <v>0</v>
-      </c>
-      <c r="V27" s="2">
-        <v>0</v>
-      </c>
-      <c r="W27" s="2">
-        <v>0</v>
-      </c>
-      <c r="X27" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="4"/>
+      <c r="J27" s="41">
+        <v>0</v>
+      </c>
+      <c r="K27" s="41">
+        <v>0</v>
+      </c>
+      <c r="L27" s="41">
+        <v>0</v>
+      </c>
+      <c r="M27" s="41">
+        <v>1</v>
+      </c>
+      <c r="N27" s="41">
+        <v>0</v>
+      </c>
+      <c r="O27" s="41">
+        <v>0</v>
+      </c>
+      <c r="P27" s="41">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="41">
+        <v>0</v>
+      </c>
+      <c r="R27" s="41">
+        <v>0</v>
+      </c>
+      <c r="S27" s="41">
+        <v>0</v>
+      </c>
+      <c r="T27" s="41">
+        <v>0</v>
+      </c>
+      <c r="U27" s="41">
+        <v>0</v>
+      </c>
+      <c r="V27" s="41">
+        <v>0</v>
+      </c>
+      <c r="W27" s="41">
+        <v>0</v>
+      </c>
+      <c r="X27" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="41">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="41">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="41">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="40"/>
       <c r="AE27" s="4"/>
       <c r="AF27" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0001200</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="14.25" customHeight="1">
@@ -3540,28 +3698,30 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J28" s="2">
         <v>0</v>
@@ -3576,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="2">
         <v>0</v>
@@ -3600,13 +3760,13 @@
         <v>0</v>
       </c>
       <c r="V28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W28" s="2">
         <v>0</v>
       </c>
       <c r="X28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y28" s="2">
         <v>0</v>
@@ -3627,7 +3787,7 @@
       <c r="AE28" s="4"/>
       <c r="AF28" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>014041B</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="14.25" customHeight="1">
@@ -3635,7 +3795,9 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C29" s="2">
         <v>0</v>
       </c>
@@ -3659,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2">
         <v>0</v>
@@ -3677,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="2">
         <v>0</v>
@@ -3722,7 +3884,7 @@
       <c r="AE29" s="4"/>
       <c r="AF29" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0001040</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="14.25" customHeight="1">
@@ -3730,18 +3892,20 @@
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="C30" s="2">
         <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2">
         <v>0</v>
@@ -3751,7 +3915,7 @@
       </c>
       <c r="I30" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J30" s="2">
         <v>0</v>
@@ -3817,7 +3981,7 @@
       <c r="AE30" s="4"/>
       <c r="AF30" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>000001C</v>
       </c>
     </row>
     <row r="31" spans="1:32" ht="14.25" customHeight="1">
@@ -3825,31 +3989,33 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="C31" s="2">
         <v>0</v>
       </c>
       <c r="D31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2">
         <v>0</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="2">
         <v>0</v>
@@ -3876,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="S31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T31" s="2">
         <v>0</v>
@@ -3912,7 +4078,7 @@
       <c r="AE31" s="4"/>
       <c r="AF31" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>000805E</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="14.25" customHeight="1">
@@ -3920,31 +4086,33 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C32" s="2">
         <v>0</v>
       </c>
       <c r="D32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
@@ -3974,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="T32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32" s="2">
         <v>0</v>
@@ -4007,7 +4175,7 @@
       <c r="AE32" s="4"/>
       <c r="AF32" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>001005F</v>
       </c>
     </row>
     <row r="33" spans="1:33" ht="14.25" customHeight="1">
@@ -4015,9 +4183,11 @@
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="C33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -4036,7 +4206,7 @@
       </c>
       <c r="I33" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J33" s="2">
         <v>0</v>
@@ -4045,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="2">
         <v>0</v>
@@ -4072,7 +4242,7 @@
         <v>0</v>
       </c>
       <c r="U33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33" s="2">
         <v>0</v>
@@ -4087,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="Z33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA33" s="2">
         <v>0</v>
@@ -4102,7 +4272,7 @@
       <c r="AE33" s="4"/>
       <c r="AF33" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0420120</v>
       </c>
     </row>
     <row r="34" spans="1:33" ht="14.25" customHeight="1">
@@ -4110,7 +4280,9 @@
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C34" s="2">
         <v>0</v>
       </c>
@@ -4191,13 +4363,13 @@
         <v>0</v>
       </c>
       <c r="AC34" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
       <c r="AF34" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="35" spans="1:33" ht="14.25" customHeight="1">
@@ -4205,9 +4377,11 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -4219,14 +4393,14 @@
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
       <c r="I35" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J35" s="2">
         <v>0</v>
@@ -4244,7 +4418,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P35" s="2">
         <v>0</v>
@@ -4256,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="S35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T35" s="2">
         <v>0</v>
@@ -4292,7 +4466,7 @@
       <c r="AE35" s="4"/>
       <c r="AF35" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0008822</v>
       </c>
     </row>
     <row r="36" spans="1:33" ht="14.25" customHeight="1">
@@ -4300,9 +4474,11 @@
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="2">
         <v>0</v>
@@ -4314,14 +4490,14 @@
         <v>0</v>
       </c>
       <c r="G36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J36" s="2">
         <v>0</v>
@@ -4336,7 +4512,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36" s="2">
         <v>0</v>
@@ -4354,7 +4530,7 @@
         <v>0</v>
       </c>
       <c r="T36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36" s="2">
         <v>0</v>
@@ -4387,7 +4563,7 @@
       <c r="AE36" s="4"/>
       <c r="AF36" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0010423</v>
       </c>
     </row>
     <row r="37" spans="1:33" ht="14.25" customHeight="1">
@@ -4395,7 +4571,9 @@
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="C37" s="2">
         <v>0</v>
       </c>
@@ -4425,7 +4603,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="2">
         <v>0</v>
@@ -4455,7 +4633,7 @@
         <v>0</v>
       </c>
       <c r="V37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W37" s="2">
         <v>0</v>
@@ -4482,7 +4660,7 @@
       <c r="AE37" s="4"/>
       <c r="AF37" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0040100</v>
       </c>
     </row>
     <row r="38" spans="1:33" ht="14.25" customHeight="1">
@@ -4490,9 +4668,11 @@
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="C38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -4501,20 +4681,20 @@
         <v>0</v>
       </c>
       <c r="F38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="2">
         <v>0</v>
       </c>
       <c r="H38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="J38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="2">
         <v>0</v>
@@ -4544,7 +4724,7 @@
         <v>0</v>
       </c>
       <c r="T38" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" s="2">
         <v>0</v>
@@ -4570,14 +4750,14 @@
       <c r="AB38" s="2">
         <v>0</v>
       </c>
-      <c r="AC38" s="18">
+      <c r="AC38" s="20">
         <v>0</v>
       </c>
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
       <c r="AF38" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0010065</v>
       </c>
     </row>
     <row r="39" spans="1:33" ht="14.25" customHeight="1">
@@ -4585,9 +4765,11 @@
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="C39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="2">
         <v>0</v>
@@ -4596,20 +4778,20 @@
         <v>0</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="2">
         <v>0</v>
       </c>
       <c r="I39" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="2">
         <v>0</v>
@@ -4636,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T39" s="2">
         <v>0</v>
@@ -4672,7 +4854,7 @@
       <c r="AE39" s="4"/>
       <c r="AF39" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0008066</v>
       </c>
       <c r="AG39" s="4" t="s">
         <v>21</v>
@@ -4683,9 +4865,11 @@
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2">
         <v>0</v>
@@ -4694,17 +4878,17 @@
         <v>0</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J40" s="2">
         <v>0</v>
@@ -4713,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" s="2">
         <v>0</v>
@@ -4740,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="U40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V40" s="2">
         <v>0</v>
@@ -4755,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="Z40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA40" s="2">
         <v>0</v>
@@ -4770,7 +4954,7 @@
       <c r="AE40" s="4"/>
       <c r="AF40" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0420127</v>
       </c>
     </row>
     <row r="41" spans="1:33" ht="14.25" customHeight="1">
@@ -4778,7 +4962,9 @@
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="C41" s="2">
         <v>0</v>
       </c>
@@ -4858,14 +5044,14 @@
       <c r="AB41" s="2">
         <v>0</v>
       </c>
-      <c r="AC41" s="2">
-        <v>0</v>
+      <c r="AC41" s="18">
+        <v>1</v>
       </c>
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
       <c r="AF41" s="7" t="str">
         <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC41, AB41),1),     BIN2HEX(_xlfn.CONCAT(AA41,Z41,Y41, X41),1),     BIN2HEX(_xlfn.CONCAT(W41,V41,U41, T41),1),     BIN2HEX(_xlfn.CONCAT(S41,R41,Q41, P41),1),     BIN2HEX(_xlfn.CONCAT(O41,N41, M41, L41),1),     BIN2HEX(_xlfn.CONCAT(K41,J41,C41,D41),1),     BIN2HEX(_xlfn.CONCAT(E41,F41,G41,H41),1) )</f>
-        <v>0000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="42" spans="1:33" ht="14.25" customHeight="1">
@@ -4873,15 +5059,17 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="C42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2">
         <v>0</v>
       </c>
       <c r="E42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="2">
         <v>0</v>
@@ -4890,14 +5078,14 @@
         <v>0</v>
       </c>
       <c r="H42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="2">
         <v>0</v>
@@ -4924,7 +5112,7 @@
         <v>0</v>
       </c>
       <c r="S42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T42" s="2">
         <v>0</v>
@@ -4939,7 +5127,7 @@
         <v>0</v>
       </c>
       <c r="X42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y42" s="2">
         <v>0</v>
@@ -4960,7 +5148,7 @@
       <c r="AE42" s="4"/>
       <c r="AF42" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0108069</v>
       </c>
     </row>
     <row r="43" spans="1:33" ht="14.25" customHeight="1">
@@ -4968,31 +5156,33 @@
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="C43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2">
         <v>0</v>
       </c>
       <c r="E43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="2">
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
@@ -5022,7 +5212,7 @@
         <v>0</v>
       </c>
       <c r="T43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U43" s="2">
         <v>0</v>
@@ -5037,7 +5227,7 @@
         <v>0</v>
       </c>
       <c r="Y43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z43" s="2">
         <v>0</v>
@@ -5055,7 +5245,7 @@
       <c r="AE43" s="4"/>
       <c r="AF43" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>021006A</v>
       </c>
     </row>
     <row r="44" spans="1:33" ht="14.25" customHeight="1">
@@ -5063,7 +5253,9 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="C44" s="2">
         <v>0</v>
       </c>
@@ -5096,7 +5288,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N44" s="2">
         <v>0</v>
@@ -5123,7 +5315,7 @@
         <v>0</v>
       </c>
       <c r="V44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44" s="2">
         <v>0</v>
@@ -5150,7 +5342,7 @@
       <c r="AE44" s="4"/>
       <c r="AF44" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0000000</v>
+        <v>0040200</v>
       </c>
     </row>
     <row r="45" spans="1:33" ht="14.25" customHeight="1">
@@ -5736,7 +5928,7 @@
     </row>
     <row r="55" spans="1:40" ht="14.25" customHeight="1">
       <c r="B55" s="21" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="C55" s="36" t="s">
         <v>40</v>
@@ -5752,10 +5944,10 @@
         <v>0</v>
       </c>
       <c r="M55" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N55" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O55" s="4">
         <v>3</v>
@@ -5790,7 +5982,7 @@
     </row>
     <row r="56" spans="1:40" ht="14.25" customHeight="1">
       <c r="B56" s="22" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="C56" s="30" t="s">
         <v>41</v>
@@ -5806,15 +5998,17 @@
         <v>B</v>
       </c>
       <c r="M56" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N56" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="O56" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="O56" s="4">
+        <v>6</v>
+      </c>
       <c r="P56" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>06</v>
       </c>
       <c r="R56" s="31"/>
       <c r="S56" s="31"/>
@@ -5842,15 +6036,17 @@
     </row>
     <row r="57" spans="1:40" ht="14.25" customHeight="1">
       <c r="M57" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N57" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="O57" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="O57" s="4">
+        <v>9</v>
+      </c>
       <c r="P57" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>09</v>
       </c>
       <c r="R57" s="31"/>
       <c r="S57" s="31"/>
@@ -5864,15 +6060,17 @@
     </row>
     <row r="58" spans="1:40" ht="14.25" customHeight="1">
       <c r="M58" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N58" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="O58" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="O58" s="4">
+        <v>12</v>
+      </c>
       <c r="P58" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>0C</v>
       </c>
       <c r="R58" s="31"/>
       <c r="S58" s="31"/>
@@ -5886,28 +6084,32 @@
     </row>
     <row r="59" spans="1:40" ht="14.25" customHeight="1">
       <c r="M59" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N59" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="O59" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="O59" s="4">
+        <v>16</v>
+      </c>
       <c r="P59" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:40" ht="14.25" customHeight="1">
       <c r="M60" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N60" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O60" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="O60" s="4">
+        <v>20</v>
+      </c>
       <c r="P60" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>14</v>
       </c>
       <c r="R60" s="32" t="s">
         <v>30</v>
@@ -5919,15 +6121,17 @@
     </row>
     <row r="61" spans="1:40" ht="14.25" customHeight="1">
       <c r="M61" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N61" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="O61" s="4"/>
+        <v>61</v>
+      </c>
+      <c r="O61" s="4">
+        <v>26</v>
+      </c>
       <c r="P61" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>1A</v>
       </c>
       <c r="R61" s="32"/>
       <c r="S61" s="32"/>
@@ -5937,15 +6141,17 @@
     </row>
     <row r="62" spans="1:40" ht="15" customHeight="1">
       <c r="M62" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N62" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="O62" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="O62" s="4">
+        <v>28</v>
+      </c>
       <c r="P62" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>1C</v>
       </c>
       <c r="R62" s="32"/>
       <c r="S62" s="32"/>
@@ -5955,15 +6161,17 @@
     </row>
     <row r="63" spans="1:40" ht="14.25" customHeight="1">
       <c r="M63" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N63" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="O63" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="O63" s="4">
+        <v>29</v>
+      </c>
       <c r="P63" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>1D</v>
       </c>
       <c r="R63" s="32"/>
       <c r="S63" s="32"/>
@@ -5973,15 +6181,17 @@
     </row>
     <row r="64" spans="1:40" ht="14.25" customHeight="1">
       <c r="M64" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N64" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="O64" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="O64" s="4">
+        <v>33</v>
+      </c>
       <c r="P64" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>21</v>
       </c>
       <c r="R64" s="32"/>
       <c r="S64" s="32"/>
@@ -5991,15 +6201,17 @@
     </row>
     <row r="65" spans="13:42" ht="14.25" customHeight="1">
       <c r="M65" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N65" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="O65" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="O65" s="4">
+        <v>36</v>
+      </c>
       <c r="P65" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>24</v>
       </c>
       <c r="R65" s="32"/>
       <c r="S65" s="32"/>
@@ -6009,28 +6221,32 @@
     </row>
     <row r="66" spans="13:42" ht="14.25" customHeight="1">
       <c r="M66" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N66" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="N66" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="O66" s="4"/>
+      <c r="O66" s="4">
+        <v>40</v>
+      </c>
       <c r="P66" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="13:42" ht="14.25" customHeight="1">
       <c r="M67" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N67" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="O67" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="O67" s="4">
+        <v>40</v>
+      </c>
       <c r="P67" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>00</v>
+        <v>28</v>
       </c>
     </row>
     <row r="68" spans="13:42" ht="14.25" customHeight="1">
@@ -7029,7 +7245,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC41 AC45:AC48 J49:AC49">
+  <conditionalFormatting sqref="AC45:AC48 J49:AC49 AC2:AC41">
     <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>